<commit_message>
updated fixtures after an issue
</commit_message>
<xml_diff>
--- a/downloads/extracted_table.xlsx
+++ b/downloads/extracted_table.xlsx
@@ -439,7 +439,7 @@
         <v>Maintenance Expenses</v>
       </c>
       <c r="B5" t="str">
-        <v>₹ 3,000</v>
+        <v>₹ 2,500</v>
       </c>
     </row>
     <row r="6">
@@ -447,7 +447,7 @@
         <v>Total Monthly Payment</v>
       </c>
       <c r="B6" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
     </row>
     <row r="7">
@@ -487,7 +487,7 @@
         <v>Taxes, Home Insurance &amp; Maintenance</v>
       </c>
       <c r="B11" t="str">
-        <v>₹ 5,10,000</v>
+        <v>₹ 4,50,000</v>
       </c>
     </row>
     <row r="12">
@@ -524,10 +524,10 @@
         <v>₹ 2,47,821</v>
       </c>
       <c r="D13" t="str">
-        <v>₹ 29,750</v>
+        <v>₹ 26,250</v>
       </c>
       <c r="E13" t="str">
-        <v>₹ 4,88,368</v>
+        <v>₹ 4,84,868</v>
       </c>
       <c r="F13" t="str">
         <v>₹ 51,89,203</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Jun₹ 29,517₹ 36,000₹ 4,250₹ 69,767₹ 53,70,4830.55%Jul₹ 29,714₹ 35,803₹ 4,250₹ 69,767₹ 53,40,7691.1%Aug₹ 29,912₹ 35,605₹ 4,250₹ 69,767₹ 53,10,8581.65%Sep₹ 30,111₹ 35,406₹ 4,250₹ 69,767₹ 52,80,7462.21%Oct₹ 30,312₹ 35,205₹ 4,250₹ 69,767₹ 52,50,4352.77%Nov₹ 30,514₹ 35,003₹ 4,250₹ 69,767₹ 52,19,9213.33%Dec₹ 30,717₹ 34,799₹ 4,250₹ 69,767₹ 51,89,2033.9%</v>
+        <v>Jun₹ 29,517₹ 36,000₹ 3,750₹ 69,267₹ 53,70,4830.55%Jul₹ 29,714₹ 35,803₹ 3,750₹ 69,267₹ 53,40,7691.1%Aug₹ 29,912₹ 35,605₹ 3,750₹ 69,267₹ 53,10,8581.65%Sep₹ 30,111₹ 35,406₹ 3,750₹ 69,267₹ 52,80,7462.21%Oct₹ 30,312₹ 35,205₹ 3,750₹ 69,267₹ 52,50,4352.77%Nov₹ 30,514₹ 35,003₹ 3,750₹ 69,267₹ 52,19,9213.33%Dec₹ 30,717₹ 34,799₹ 3,750₹ 69,267₹ 51,89,2033.9%</v>
       </c>
       <c r="B14" t="str">
         <v>Jun</v>
@@ -550,10 +550,10 @@
         <v>₹ 36,000</v>
       </c>
       <c r="E14" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F14" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G14" t="str">
         <v>₹ 53,70,483</v>
@@ -571,10 +571,10 @@
         <v>₹ 35,803</v>
       </c>
       <c r="L14" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M14" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N14" t="str">
         <v>₹ 53,40,769</v>
@@ -592,10 +592,10 @@
         <v>₹ 35,605</v>
       </c>
       <c r="S14" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T14" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U14" t="str">
         <v>₹ 53,10,858</v>
@@ -613,10 +613,10 @@
         <v>₹ 35,406</v>
       </c>
       <c r="Z14" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA14" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB14" t="str">
         <v>₹ 52,80,746</v>
@@ -634,10 +634,10 @@
         <v>₹ 35,205</v>
       </c>
       <c r="AG14" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH14" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI14" t="str">
         <v>₹ 52,50,435</v>
@@ -655,10 +655,10 @@
         <v>₹ 35,003</v>
       </c>
       <c r="AN14" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO14" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP14" t="str">
         <v>₹ 52,19,921</v>
@@ -676,10 +676,10 @@
         <v>₹ 34,799</v>
       </c>
       <c r="AU14" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV14" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW14" t="str">
         <v>₹ 51,89,203</v>
@@ -699,10 +699,10 @@
         <v>₹ 36,000</v>
       </c>
       <c r="D15" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E15" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F15" t="str">
         <v>₹ 53,70,483</v>
@@ -722,10 +722,10 @@
         <v>₹ 35,803</v>
       </c>
       <c r="D16" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E16" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F16" t="str">
         <v>₹ 53,40,769</v>
@@ -745,10 +745,10 @@
         <v>₹ 35,605</v>
       </c>
       <c r="D17" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E17" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F17" t="str">
         <v>₹ 53,10,858</v>
@@ -768,10 +768,10 @@
         <v>₹ 35,406</v>
       </c>
       <c r="D18" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E18" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F18" t="str">
         <v>₹ 52,80,746</v>
@@ -791,10 +791,10 @@
         <v>₹ 35,205</v>
       </c>
       <c r="D19" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E19" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F19" t="str">
         <v>₹ 52,50,435</v>
@@ -814,10 +814,10 @@
         <v>₹ 35,003</v>
       </c>
       <c r="D20" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E20" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F20" t="str">
         <v>₹ 52,19,921</v>
@@ -837,10 +837,10 @@
         <v>₹ 34,799</v>
       </c>
       <c r="D21" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E21" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F21" t="str">
         <v>₹ 51,89,203</v>
@@ -860,10 +860,10 @@
         <v>₹ 4,01,224</v>
       </c>
       <c r="D22" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E22" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F22" t="str">
         <v>₹ 48,04,224</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Jan₹ 30,922₹ 34,595₹ 4,250₹ 69,767₹ 51,58,2814.48%Feb₹ 31,128₹ 34,389₹ 4,250₹ 69,767₹ 51,27,1535.05%Mar₹ 31,336₹ 34,181₹ 4,250₹ 69,767₹ 50,95,8175.63%Apr₹ 31,545₹ 33,972₹ 4,250₹ 69,767₹ 50,64,2726.22%May₹ 31,755₹ 33,762₹ 4,250₹ 69,767₹ 50,32,5176.81%Jun₹ 31,967₹ 33,550₹ 4,250₹ 69,767₹ 50,00,5507.4%Jul₹ 32,180₹ 33,337₹ 4,250₹ 69,767₹ 49,68,3707.99%Aug₹ 32,394₹ 33,122₹ 4,250₹ 69,767₹ 49,35,9768.59%Sep₹ 32,610₹ 32,907₹ 4,250₹ 69,767₹ 49,03,3659.2%Oct₹ 32,828₹ 32,689₹ 4,250₹ 69,767₹ 48,70,5379.8%Nov₹ 33,047₹ 32,470₹ 4,250₹ 69,767₹ 48,37,49110.42%Dec₹ 33,267₹ 32,250₹ 4,250₹ 69,767₹ 48,04,22411.03%</v>
+        <v>Jan₹ 30,922₹ 34,595₹ 3,750₹ 69,267₹ 51,58,2814.48%Feb₹ 31,128₹ 34,389₹ 3,750₹ 69,267₹ 51,27,1535.05%Mar₹ 31,336₹ 34,181₹ 3,750₹ 69,267₹ 50,95,8175.63%Apr₹ 31,545₹ 33,972₹ 3,750₹ 69,267₹ 50,64,2726.22%May₹ 31,755₹ 33,762₹ 3,750₹ 69,267₹ 50,32,5176.81%Jun₹ 31,967₹ 33,550₹ 3,750₹ 69,267₹ 50,00,5507.4%Jul₹ 32,180₹ 33,337₹ 3,750₹ 69,267₹ 49,68,3707.99%Aug₹ 32,394₹ 33,122₹ 3,750₹ 69,267₹ 49,35,9768.59%Sep₹ 32,610₹ 32,907₹ 3,750₹ 69,267₹ 49,03,3659.2%Oct₹ 32,828₹ 32,689₹ 3,750₹ 69,267₹ 48,70,5379.8%Nov₹ 33,047₹ 32,470₹ 3,750₹ 69,267₹ 48,37,49110.42%Dec₹ 33,267₹ 32,250₹ 3,750₹ 69,267₹ 48,04,22411.03%</v>
       </c>
       <c r="B23" t="str">
         <v>Jan</v>
@@ -886,10 +886,10 @@
         <v>₹ 34,595</v>
       </c>
       <c r="E23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G23" t="str">
         <v>₹ 51,58,281</v>
@@ -907,10 +907,10 @@
         <v>₹ 34,389</v>
       </c>
       <c r="L23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N23" t="str">
         <v>₹ 51,27,153</v>
@@ -928,10 +928,10 @@
         <v>₹ 34,181</v>
       </c>
       <c r="S23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U23" t="str">
         <v>₹ 50,95,817</v>
@@ -949,10 +949,10 @@
         <v>₹ 33,972</v>
       </c>
       <c r="Z23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB23" t="str">
         <v>₹ 50,64,272</v>
@@ -970,10 +970,10 @@
         <v>₹ 33,762</v>
       </c>
       <c r="AG23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI23" t="str">
         <v>₹ 50,32,517</v>
@@ -991,10 +991,10 @@
         <v>₹ 33,550</v>
       </c>
       <c r="AN23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP23" t="str">
         <v>₹ 50,00,550</v>
@@ -1012,10 +1012,10 @@
         <v>₹ 33,337</v>
       </c>
       <c r="AU23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW23" t="str">
         <v>₹ 49,68,370</v>
@@ -1033,10 +1033,10 @@
         <v>₹ 33,122</v>
       </c>
       <c r="BB23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD23" t="str">
         <v>₹ 49,35,976</v>
@@ -1054,10 +1054,10 @@
         <v>₹ 32,907</v>
       </c>
       <c r="BI23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK23" t="str">
         <v>₹ 49,03,365</v>
@@ -1075,10 +1075,10 @@
         <v>₹ 32,689</v>
       </c>
       <c r="BP23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR23" t="str">
         <v>₹ 48,70,537</v>
@@ -1096,10 +1096,10 @@
         <v>₹ 32,470</v>
       </c>
       <c r="BW23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY23" t="str">
         <v>₹ 48,37,491</v>
@@ -1117,10 +1117,10 @@
         <v>₹ 32,250</v>
       </c>
       <c r="CD23" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE23" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF23" t="str">
         <v>₹ 48,04,224</v>
@@ -1140,10 +1140,10 @@
         <v>₹ 34,595</v>
       </c>
       <c r="D24" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E24" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F24" t="str">
         <v>₹ 51,58,281</v>
@@ -1163,10 +1163,10 @@
         <v>₹ 34,389</v>
       </c>
       <c r="D25" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E25" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F25" t="str">
         <v>₹ 51,27,153</v>
@@ -1186,10 +1186,10 @@
         <v>₹ 34,181</v>
       </c>
       <c r="D26" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E26" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F26" t="str">
         <v>₹ 50,95,817</v>
@@ -1209,10 +1209,10 @@
         <v>₹ 33,972</v>
       </c>
       <c r="D27" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E27" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F27" t="str">
         <v>₹ 50,64,272</v>
@@ -1232,10 +1232,10 @@
         <v>₹ 33,762</v>
       </c>
       <c r="D28" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E28" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F28" t="str">
         <v>₹ 50,32,517</v>
@@ -1255,10 +1255,10 @@
         <v>₹ 33,550</v>
       </c>
       <c r="D29" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E29" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F29" t="str">
         <v>₹ 50,00,550</v>
@@ -1278,10 +1278,10 @@
         <v>₹ 33,337</v>
       </c>
       <c r="D30" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E30" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F30" t="str">
         <v>₹ 49,68,370</v>
@@ -1301,10 +1301,10 @@
         <v>₹ 33,122</v>
       </c>
       <c r="D31" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E31" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F31" t="str">
         <v>₹ 49,35,976</v>
@@ -1324,10 +1324,10 @@
         <v>₹ 32,907</v>
       </c>
       <c r="D32" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E32" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F32" t="str">
         <v>₹ 49,03,365</v>
@@ -1347,10 +1347,10 @@
         <v>₹ 32,689</v>
       </c>
       <c r="D33" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E33" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F33" t="str">
         <v>₹ 48,70,537</v>
@@ -1370,10 +1370,10 @@
         <v>₹ 32,470</v>
       </c>
       <c r="D34" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E34" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F34" t="str">
         <v>₹ 48,37,491</v>
@@ -1393,10 +1393,10 @@
         <v>₹ 32,250</v>
       </c>
       <c r="D35" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E35" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F35" t="str">
         <v>₹ 48,04,224</v>
@@ -1416,10 +1416,10 @@
         <v>₹ 3,69,270</v>
       </c>
       <c r="D36" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E36" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F36" t="str">
         <v>₹ 43,87,291</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Jan₹ 33,489₹ 32,028₹ 4,250₹ 69,767₹ 47,70,73511.65%Feb₹ 33,712₹ 31,805₹ 4,250₹ 69,767₹ 47,37,02312.28%Mar₹ 33,937₹ 31,580₹ 4,250₹ 69,767₹ 47,03,08612.91%Apr₹ 34,163₹ 31,354₹ 4,250₹ 69,767₹ 46,68,92313.54%May₹ 34,391₹ 31,126₹ 4,250₹ 69,767₹ 46,34,53314.18%Jun₹ 34,620₹ 30,897₹ 4,250₹ 69,767₹ 45,99,91314.82%Jul₹ 34,851₹ 30,666₹ 4,250₹ 69,767₹ 45,65,06215.46%Aug₹ 35,083₹ 30,434₹ 4,250₹ 69,767₹ 45,29,97916.11%Sep₹ 35,317₹ 30,200₹ 4,250₹ 69,767₹ 44,94,66216.77%Oct₹ 35,552₹ 29,964₹ 4,250₹ 69,767₹ 44,59,10917.42%Nov₹ 35,790₹ 29,727₹ 4,250₹ 69,767₹ 44,23,32018.09%Dec₹ 36,028₹ 29,489₹ 4,250₹ 69,767₹ 43,87,29118.75%</v>
+        <v>Jan₹ 33,489₹ 32,028₹ 3,750₹ 69,267₹ 47,70,73511.65%Feb₹ 33,712₹ 31,805₹ 3,750₹ 69,267₹ 47,37,02312.28%Mar₹ 33,937₹ 31,580₹ 3,750₹ 69,267₹ 47,03,08612.91%Apr₹ 34,163₹ 31,354₹ 3,750₹ 69,267₹ 46,68,92313.54%May₹ 34,391₹ 31,126₹ 3,750₹ 69,267₹ 46,34,53314.18%Jun₹ 34,620₹ 30,897₹ 3,750₹ 69,267₹ 45,99,91314.82%Jul₹ 34,851₹ 30,666₹ 3,750₹ 69,267₹ 45,65,06215.46%Aug₹ 35,083₹ 30,434₹ 3,750₹ 69,267₹ 45,29,97916.11%Sep₹ 35,317₹ 30,200₹ 3,750₹ 69,267₹ 44,94,66216.77%Oct₹ 35,552₹ 29,964₹ 3,750₹ 69,267₹ 44,59,10917.42%Nov₹ 35,790₹ 29,727₹ 3,750₹ 69,267₹ 44,23,32018.09%Dec₹ 36,028₹ 29,489₹ 3,750₹ 69,267₹ 43,87,29118.75%</v>
       </c>
       <c r="B37" t="str">
         <v>Jan</v>
@@ -1442,10 +1442,10 @@
         <v>₹ 32,028</v>
       </c>
       <c r="E37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G37" t="str">
         <v>₹ 47,70,735</v>
@@ -1463,10 +1463,10 @@
         <v>₹ 31,805</v>
       </c>
       <c r="L37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N37" t="str">
         <v>₹ 47,37,023</v>
@@ -1484,10 +1484,10 @@
         <v>₹ 31,580</v>
       </c>
       <c r="S37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U37" t="str">
         <v>₹ 47,03,086</v>
@@ -1505,10 +1505,10 @@
         <v>₹ 31,354</v>
       </c>
       <c r="Z37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB37" t="str">
         <v>₹ 46,68,923</v>
@@ -1526,10 +1526,10 @@
         <v>₹ 31,126</v>
       </c>
       <c r="AG37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI37" t="str">
         <v>₹ 46,34,533</v>
@@ -1547,10 +1547,10 @@
         <v>₹ 30,897</v>
       </c>
       <c r="AN37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP37" t="str">
         <v>₹ 45,99,913</v>
@@ -1568,10 +1568,10 @@
         <v>₹ 30,666</v>
       </c>
       <c r="AU37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW37" t="str">
         <v>₹ 45,65,062</v>
@@ -1589,10 +1589,10 @@
         <v>₹ 30,434</v>
       </c>
       <c r="BB37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD37" t="str">
         <v>₹ 45,29,979</v>
@@ -1610,10 +1610,10 @@
         <v>₹ 30,200</v>
       </c>
       <c r="BI37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK37" t="str">
         <v>₹ 44,94,662</v>
@@ -1631,10 +1631,10 @@
         <v>₹ 29,964</v>
       </c>
       <c r="BP37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR37" t="str">
         <v>₹ 44,59,109</v>
@@ -1652,10 +1652,10 @@
         <v>₹ 29,727</v>
       </c>
       <c r="BW37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY37" t="str">
         <v>₹ 44,23,320</v>
@@ -1673,10 +1673,10 @@
         <v>₹ 29,489</v>
       </c>
       <c r="CD37" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE37" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF37" t="str">
         <v>₹ 43,87,291</v>
@@ -1696,10 +1696,10 @@
         <v>₹ 32,028</v>
       </c>
       <c r="D38" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E38" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F38" t="str">
         <v>₹ 47,70,735</v>
@@ -1719,10 +1719,10 @@
         <v>₹ 31,805</v>
       </c>
       <c r="D39" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E39" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F39" t="str">
         <v>₹ 47,37,023</v>
@@ -1742,10 +1742,10 @@
         <v>₹ 31,580</v>
       </c>
       <c r="D40" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E40" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F40" t="str">
         <v>₹ 47,03,086</v>
@@ -1765,10 +1765,10 @@
         <v>₹ 31,354</v>
       </c>
       <c r="D41" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E41" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F41" t="str">
         <v>₹ 46,68,923</v>
@@ -1788,10 +1788,10 @@
         <v>₹ 31,126</v>
       </c>
       <c r="D42" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E42" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F42" t="str">
         <v>₹ 46,34,533</v>
@@ -1811,10 +1811,10 @@
         <v>₹ 30,897</v>
       </c>
       <c r="D43" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E43" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F43" t="str">
         <v>₹ 45,99,913</v>
@@ -1834,10 +1834,10 @@
         <v>₹ 30,666</v>
       </c>
       <c r="D44" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E44" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F44" t="str">
         <v>₹ 45,65,062</v>
@@ -1857,10 +1857,10 @@
         <v>₹ 30,434</v>
       </c>
       <c r="D45" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E45" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F45" t="str">
         <v>₹ 45,29,979</v>
@@ -1880,10 +1880,10 @@
         <v>₹ 30,200</v>
       </c>
       <c r="D46" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E46" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F46" t="str">
         <v>₹ 44,94,662</v>
@@ -1903,10 +1903,10 @@
         <v>₹ 29,964</v>
       </c>
       <c r="D47" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E47" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F47" t="str">
         <v>₹ 44,59,109</v>
@@ -1926,10 +1926,10 @@
         <v>₹ 29,727</v>
       </c>
       <c r="D48" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E48" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F48" t="str">
         <v>₹ 44,23,320</v>
@@ -1949,10 +1949,10 @@
         <v>₹ 29,489</v>
       </c>
       <c r="D49" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E49" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F49" t="str">
         <v>₹ 43,87,291</v>
@@ -1972,10 +1972,10 @@
         <v>₹ 3,34,665</v>
       </c>
       <c r="D50" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E50" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F50" t="str">
         <v>₹ 39,35,754</v>
@@ -1986,7 +1986,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Jan₹ 36,268₹ 29,249₹ 4,250₹ 69,767₹ 43,51,02319.43%Feb₹ 36,510₹ 29,007₹ 4,250₹ 69,767₹ 43,14,51320.1%Mar₹ 36,753₹ 28,763₹ 4,250₹ 69,767₹ 42,77,76020.78%Apr₹ 36,999₹ 28,518₹ 4,250₹ 69,767₹ 42,40,76121.47%May₹ 37,245₹ 28,272₹ 4,250₹ 69,767₹ 42,03,51622.16%Jun₹ 37,493₹ 28,023₹ 4,250₹ 69,767₹ 41,66,02222.85%Jul₹ 37,743₹ 27,773₹ 4,250₹ 69,767₹ 41,28,27923.55%Aug₹ 37,995₹ 27,522₹ 4,250₹ 69,767₹ 40,90,28424.25%Sep₹ 38,248₹ 27,269₹ 4,250₹ 69,767₹ 40,52,03624.96%Oct₹ 38,503₹ 27,014₹ 4,250₹ 69,767₹ 40,13,53225.68%Nov₹ 38,760₹ 26,757₹ 4,250₹ 69,767₹ 39,74,77226.39%Dec₹ 39,018₹ 26,498₹ 4,250₹ 69,767₹ 39,35,75427.12%</v>
+        <v>Jan₹ 36,268₹ 29,249₹ 3,750₹ 69,267₹ 43,51,02319.43%Feb₹ 36,510₹ 29,007₹ 3,750₹ 69,267₹ 43,14,51320.1%Mar₹ 36,753₹ 28,763₹ 3,750₹ 69,267₹ 42,77,76020.78%Apr₹ 36,999₹ 28,518₹ 3,750₹ 69,267₹ 42,40,76121.47%May₹ 37,245₹ 28,272₹ 3,750₹ 69,267₹ 42,03,51622.16%Jun₹ 37,493₹ 28,023₹ 3,750₹ 69,267₹ 41,66,02222.85%Jul₹ 37,743₹ 27,773₹ 3,750₹ 69,267₹ 41,28,27923.55%Aug₹ 37,995₹ 27,522₹ 3,750₹ 69,267₹ 40,90,28424.25%Sep₹ 38,248₹ 27,269₹ 3,750₹ 69,267₹ 40,52,03624.96%Oct₹ 38,503₹ 27,014₹ 3,750₹ 69,267₹ 40,13,53225.68%Nov₹ 38,760₹ 26,757₹ 3,750₹ 69,267₹ 39,74,77226.39%Dec₹ 39,018₹ 26,498₹ 3,750₹ 69,267₹ 39,35,75427.12%</v>
       </c>
       <c r="B51" t="str">
         <v>Jan</v>
@@ -1998,10 +1998,10 @@
         <v>₹ 29,249</v>
       </c>
       <c r="E51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G51" t="str">
         <v>₹ 43,51,023</v>
@@ -2019,10 +2019,10 @@
         <v>₹ 29,007</v>
       </c>
       <c r="L51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N51" t="str">
         <v>₹ 43,14,513</v>
@@ -2040,10 +2040,10 @@
         <v>₹ 28,763</v>
       </c>
       <c r="S51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U51" t="str">
         <v>₹ 42,77,760</v>
@@ -2061,10 +2061,10 @@
         <v>₹ 28,518</v>
       </c>
       <c r="Z51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB51" t="str">
         <v>₹ 42,40,761</v>
@@ -2082,10 +2082,10 @@
         <v>₹ 28,272</v>
       </c>
       <c r="AG51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI51" t="str">
         <v>₹ 42,03,516</v>
@@ -2103,10 +2103,10 @@
         <v>₹ 28,023</v>
       </c>
       <c r="AN51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP51" t="str">
         <v>₹ 41,66,022</v>
@@ -2124,10 +2124,10 @@
         <v>₹ 27,773</v>
       </c>
       <c r="AU51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW51" t="str">
         <v>₹ 41,28,279</v>
@@ -2145,10 +2145,10 @@
         <v>₹ 27,522</v>
       </c>
       <c r="BB51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD51" t="str">
         <v>₹ 40,90,284</v>
@@ -2166,10 +2166,10 @@
         <v>₹ 27,269</v>
       </c>
       <c r="BI51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK51" t="str">
         <v>₹ 40,52,036</v>
@@ -2187,10 +2187,10 @@
         <v>₹ 27,014</v>
       </c>
       <c r="BP51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR51" t="str">
         <v>₹ 40,13,532</v>
@@ -2208,10 +2208,10 @@
         <v>₹ 26,757</v>
       </c>
       <c r="BW51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY51" t="str">
         <v>₹ 39,74,772</v>
@@ -2229,10 +2229,10 @@
         <v>₹ 26,498</v>
       </c>
       <c r="CD51" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE51" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF51" t="str">
         <v>₹ 39,35,754</v>
@@ -2252,10 +2252,10 @@
         <v>₹ 29,249</v>
       </c>
       <c r="D52" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E52" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F52" t="str">
         <v>₹ 43,51,023</v>
@@ -2275,10 +2275,10 @@
         <v>₹ 29,007</v>
       </c>
       <c r="D53" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E53" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F53" t="str">
         <v>₹ 43,14,513</v>
@@ -2298,10 +2298,10 @@
         <v>₹ 28,763</v>
       </c>
       <c r="D54" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E54" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F54" t="str">
         <v>₹ 42,77,760</v>
@@ -2321,10 +2321,10 @@
         <v>₹ 28,518</v>
       </c>
       <c r="D55" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E55" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F55" t="str">
         <v>₹ 42,40,761</v>
@@ -2344,10 +2344,10 @@
         <v>₹ 28,272</v>
       </c>
       <c r="D56" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E56" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F56" t="str">
         <v>₹ 42,03,516</v>
@@ -2367,10 +2367,10 @@
         <v>₹ 28,023</v>
       </c>
       <c r="D57" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E57" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F57" t="str">
         <v>₹ 41,66,022</v>
@@ -2390,10 +2390,10 @@
         <v>₹ 27,773</v>
       </c>
       <c r="D58" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E58" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F58" t="str">
         <v>₹ 41,28,279</v>
@@ -2413,10 +2413,10 @@
         <v>₹ 27,522</v>
       </c>
       <c r="D59" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E59" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F59" t="str">
         <v>₹ 40,90,284</v>
@@ -2436,10 +2436,10 @@
         <v>₹ 27,269</v>
       </c>
       <c r="D60" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E60" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F60" t="str">
         <v>₹ 40,52,036</v>
@@ -2459,10 +2459,10 @@
         <v>₹ 27,014</v>
       </c>
       <c r="D61" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E61" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F61" t="str">
         <v>₹ 40,13,532</v>
@@ -2482,10 +2482,10 @@
         <v>₹ 26,757</v>
       </c>
       <c r="D62" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E62" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F62" t="str">
         <v>₹ 39,74,772</v>
@@ -2505,10 +2505,10 @@
         <v>₹ 26,498</v>
       </c>
       <c r="D63" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E63" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F63" t="str">
         <v>₹ 39,35,754</v>
@@ -2528,10 +2528,10 @@
         <v>₹ 2,97,188</v>
       </c>
       <c r="D64" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E64" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F64" t="str">
         <v>₹ 34,46,739</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Jan₹ 39,279₹ 26,238₹ 4,250₹ 69,767₹ 38,96,47527.84%Feb₹ 39,540₹ 25,977₹ 4,250₹ 69,767₹ 38,56,93528.58%Mar₹ 39,804₹ 25,713₹ 4,250₹ 69,767₹ 38,17,13129.31%Apr₹ 40,069₹ 25,448₹ 4,250₹ 69,767₹ 37,77,06230.05%May₹ 40,336₹ 25,180₹ 4,250₹ 69,767₹ 37,36,72530.8%Jun₹ 40,605₹ 24,912₹ 4,250₹ 69,767₹ 36,96,12031.55%Jul₹ 40,876₹ 24,641₹ 4,250₹ 69,767₹ 36,55,24432.31%Aug₹ 41,149₹ 24,368₹ 4,250₹ 69,767₹ 36,14,09533.07%Sep₹ 41,423₹ 24,094₹ 4,250₹ 69,767₹ 35,72,67233.84%Oct₹ 41,699₹ 23,818₹ 4,250₹ 69,767₹ 35,30,97334.61%Nov₹ 41,977₹ 23,540₹ 4,250₹ 69,767₹ 34,88,99635.39%Dec₹ 42,257₹ 23,260₹ 4,250₹ 69,767₹ 34,46,73936.17%</v>
+        <v>Jan₹ 39,279₹ 26,238₹ 3,750₹ 69,267₹ 38,96,47527.84%Feb₹ 39,540₹ 25,977₹ 3,750₹ 69,267₹ 38,56,93528.58%Mar₹ 39,804₹ 25,713₹ 3,750₹ 69,267₹ 38,17,13129.31%Apr₹ 40,069₹ 25,448₹ 3,750₹ 69,267₹ 37,77,06230.05%May₹ 40,336₹ 25,180₹ 3,750₹ 69,267₹ 37,36,72530.8%Jun₹ 40,605₹ 24,912₹ 3,750₹ 69,267₹ 36,96,12031.55%Jul₹ 40,876₹ 24,641₹ 3,750₹ 69,267₹ 36,55,24432.31%Aug₹ 41,149₹ 24,368₹ 3,750₹ 69,267₹ 36,14,09533.07%Sep₹ 41,423₹ 24,094₹ 3,750₹ 69,267₹ 35,72,67233.84%Oct₹ 41,699₹ 23,818₹ 3,750₹ 69,267₹ 35,30,97334.61%Nov₹ 41,977₹ 23,540₹ 3,750₹ 69,267₹ 34,88,99635.39%Dec₹ 42,257₹ 23,260₹ 3,750₹ 69,267₹ 34,46,73936.17%</v>
       </c>
       <c r="B65" t="str">
         <v>Jan</v>
@@ -2554,10 +2554,10 @@
         <v>₹ 26,238</v>
       </c>
       <c r="E65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G65" t="str">
         <v>₹ 38,96,475</v>
@@ -2575,10 +2575,10 @@
         <v>₹ 25,977</v>
       </c>
       <c r="L65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N65" t="str">
         <v>₹ 38,56,935</v>
@@ -2596,10 +2596,10 @@
         <v>₹ 25,713</v>
       </c>
       <c r="S65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U65" t="str">
         <v>₹ 38,17,131</v>
@@ -2617,10 +2617,10 @@
         <v>₹ 25,448</v>
       </c>
       <c r="Z65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB65" t="str">
         <v>₹ 37,77,062</v>
@@ -2638,10 +2638,10 @@
         <v>₹ 25,180</v>
       </c>
       <c r="AG65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI65" t="str">
         <v>₹ 37,36,725</v>
@@ -2659,10 +2659,10 @@
         <v>₹ 24,912</v>
       </c>
       <c r="AN65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP65" t="str">
         <v>₹ 36,96,120</v>
@@ -2680,10 +2680,10 @@
         <v>₹ 24,641</v>
       </c>
       <c r="AU65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW65" t="str">
         <v>₹ 36,55,244</v>
@@ -2701,10 +2701,10 @@
         <v>₹ 24,368</v>
       </c>
       <c r="BB65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD65" t="str">
         <v>₹ 36,14,095</v>
@@ -2722,10 +2722,10 @@
         <v>₹ 24,094</v>
       </c>
       <c r="BI65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK65" t="str">
         <v>₹ 35,72,672</v>
@@ -2743,10 +2743,10 @@
         <v>₹ 23,818</v>
       </c>
       <c r="BP65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR65" t="str">
         <v>₹ 35,30,973</v>
@@ -2764,10 +2764,10 @@
         <v>₹ 23,540</v>
       </c>
       <c r="BW65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY65" t="str">
         <v>₹ 34,88,996</v>
@@ -2785,10 +2785,10 @@
         <v>₹ 23,260</v>
       </c>
       <c r="CD65" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE65" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF65" t="str">
         <v>₹ 34,46,739</v>
@@ -2808,10 +2808,10 @@
         <v>₹ 26,238</v>
       </c>
       <c r="D66" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E66" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F66" t="str">
         <v>₹ 38,96,475</v>
@@ -2831,10 +2831,10 @@
         <v>₹ 25,977</v>
       </c>
       <c r="D67" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E67" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F67" t="str">
         <v>₹ 38,56,935</v>
@@ -2854,10 +2854,10 @@
         <v>₹ 25,713</v>
       </c>
       <c r="D68" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E68" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F68" t="str">
         <v>₹ 38,17,131</v>
@@ -2877,10 +2877,10 @@
         <v>₹ 25,448</v>
       </c>
       <c r="D69" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E69" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F69" t="str">
         <v>₹ 37,77,062</v>
@@ -2900,10 +2900,10 @@
         <v>₹ 25,180</v>
       </c>
       <c r="D70" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E70" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F70" t="str">
         <v>₹ 37,36,725</v>
@@ -2923,10 +2923,10 @@
         <v>₹ 24,912</v>
       </c>
       <c r="D71" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E71" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F71" t="str">
         <v>₹ 36,96,120</v>
@@ -2946,10 +2946,10 @@
         <v>₹ 24,641</v>
       </c>
       <c r="D72" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E72" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F72" t="str">
         <v>₹ 36,55,244</v>
@@ -2969,10 +2969,10 @@
         <v>₹ 24,368</v>
       </c>
       <c r="D73" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E73" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F73" t="str">
         <v>₹ 36,14,095</v>
@@ -2992,10 +2992,10 @@
         <v>₹ 24,094</v>
       </c>
       <c r="D74" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E74" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F74" t="str">
         <v>₹ 35,72,672</v>
@@ -3015,10 +3015,10 @@
         <v>₹ 23,818</v>
       </c>
       <c r="D75" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E75" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F75" t="str">
         <v>₹ 35,30,973</v>
@@ -3038,10 +3038,10 @@
         <v>₹ 23,540</v>
       </c>
       <c r="D76" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E76" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F76" t="str">
         <v>₹ 34,88,996</v>
@@ -3061,10 +3061,10 @@
         <v>₹ 23,260</v>
       </c>
       <c r="D77" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E77" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F77" t="str">
         <v>₹ 34,46,739</v>
@@ -3084,10 +3084,10 @@
         <v>₹ 2,56,600</v>
       </c>
       <c r="D78" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E78" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F78" t="str">
         <v>₹ 29,17,136</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>Jan₹ 42,539₹ 22,978₹ 4,250₹ 69,767₹ 34,04,20036.96%Feb₹ 42,822₹ 22,695₹ 4,250₹ 69,767₹ 33,61,37837.75%Mar₹ 43,108₹ 22,409₹ 4,250₹ 69,767₹ 33,18,27038.55%Apr₹ 43,395₹ 22,122₹ 4,250₹ 69,767₹ 32,74,87539.35%May₹ 43,684₹ 21,833₹ 4,250₹ 69,767₹ 32,31,19140.16%Jun₹ 43,976₹ 21,541₹ 4,250₹ 69,767₹ 31,87,21540.98%Jul₹ 44,269₹ 21,248₹ 4,250₹ 69,767₹ 31,42,94641.8%Aug₹ 44,564₹ 20,953₹ 4,250₹ 69,767₹ 30,98,38342.62%Sep₹ 44,861₹ 20,656₹ 4,250₹ 69,767₹ 30,53,52243.45%Oct₹ 45,160₹ 20,357₹ 4,250₹ 69,767₹ 30,08,36144.29%Nov₹ 45,461₹ 20,056₹ 4,250₹ 69,767₹ 29,62,90045.13%Dec₹ 45,764₹ 19,753₹ 4,250₹ 69,767₹ 29,17,13645.98%</v>
+        <v>Jan₹ 42,539₹ 22,978₹ 3,750₹ 69,267₹ 34,04,20036.96%Feb₹ 42,822₹ 22,695₹ 3,750₹ 69,267₹ 33,61,37837.75%Mar₹ 43,108₹ 22,409₹ 3,750₹ 69,267₹ 33,18,27038.55%Apr₹ 43,395₹ 22,122₹ 3,750₹ 69,267₹ 32,74,87539.35%May₹ 43,684₹ 21,833₹ 3,750₹ 69,267₹ 32,31,19140.16%Jun₹ 43,976₹ 21,541₹ 3,750₹ 69,267₹ 31,87,21540.98%Jul₹ 44,269₹ 21,248₹ 3,750₹ 69,267₹ 31,42,94641.8%Aug₹ 44,564₹ 20,953₹ 3,750₹ 69,267₹ 30,98,38342.62%Sep₹ 44,861₹ 20,656₹ 3,750₹ 69,267₹ 30,53,52243.45%Oct₹ 45,160₹ 20,357₹ 3,750₹ 69,267₹ 30,08,36144.29%Nov₹ 45,461₹ 20,056₹ 3,750₹ 69,267₹ 29,62,90045.13%Dec₹ 45,764₹ 19,753₹ 3,750₹ 69,267₹ 29,17,13645.98%</v>
       </c>
       <c r="B79" t="str">
         <v>Jan</v>
@@ -3110,10 +3110,10 @@
         <v>₹ 22,978</v>
       </c>
       <c r="E79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G79" t="str">
         <v>₹ 34,04,200</v>
@@ -3131,10 +3131,10 @@
         <v>₹ 22,695</v>
       </c>
       <c r="L79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N79" t="str">
         <v>₹ 33,61,378</v>
@@ -3152,10 +3152,10 @@
         <v>₹ 22,409</v>
       </c>
       <c r="S79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U79" t="str">
         <v>₹ 33,18,270</v>
@@ -3173,10 +3173,10 @@
         <v>₹ 22,122</v>
       </c>
       <c r="Z79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB79" t="str">
         <v>₹ 32,74,875</v>
@@ -3194,10 +3194,10 @@
         <v>₹ 21,833</v>
       </c>
       <c r="AG79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI79" t="str">
         <v>₹ 32,31,191</v>
@@ -3215,10 +3215,10 @@
         <v>₹ 21,541</v>
       </c>
       <c r="AN79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP79" t="str">
         <v>₹ 31,87,215</v>
@@ -3236,10 +3236,10 @@
         <v>₹ 21,248</v>
       </c>
       <c r="AU79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW79" t="str">
         <v>₹ 31,42,946</v>
@@ -3257,10 +3257,10 @@
         <v>₹ 20,953</v>
       </c>
       <c r="BB79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD79" t="str">
         <v>₹ 30,98,383</v>
@@ -3278,10 +3278,10 @@
         <v>₹ 20,656</v>
       </c>
       <c r="BI79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK79" t="str">
         <v>₹ 30,53,522</v>
@@ -3299,10 +3299,10 @@
         <v>₹ 20,357</v>
       </c>
       <c r="BP79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR79" t="str">
         <v>₹ 30,08,361</v>
@@ -3320,10 +3320,10 @@
         <v>₹ 20,056</v>
       </c>
       <c r="BW79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY79" t="str">
         <v>₹ 29,62,900</v>
@@ -3341,10 +3341,10 @@
         <v>₹ 19,753</v>
       </c>
       <c r="CD79" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE79" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF79" t="str">
         <v>₹ 29,17,136</v>
@@ -3364,10 +3364,10 @@
         <v>₹ 22,978</v>
       </c>
       <c r="D80" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E80" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F80" t="str">
         <v>₹ 34,04,200</v>
@@ -3387,10 +3387,10 @@
         <v>₹ 22,695</v>
       </c>
       <c r="D81" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E81" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F81" t="str">
         <v>₹ 33,61,378</v>
@@ -3410,10 +3410,10 @@
         <v>₹ 22,409</v>
       </c>
       <c r="D82" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E82" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F82" t="str">
         <v>₹ 33,18,270</v>
@@ -3433,10 +3433,10 @@
         <v>₹ 22,122</v>
       </c>
       <c r="D83" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E83" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F83" t="str">
         <v>₹ 32,74,875</v>
@@ -3456,10 +3456,10 @@
         <v>₹ 21,833</v>
       </c>
       <c r="D84" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E84" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F84" t="str">
         <v>₹ 32,31,191</v>
@@ -3479,10 +3479,10 @@
         <v>₹ 21,541</v>
       </c>
       <c r="D85" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E85" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F85" t="str">
         <v>₹ 31,87,215</v>
@@ -3502,10 +3502,10 @@
         <v>₹ 21,248</v>
       </c>
       <c r="D86" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E86" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F86" t="str">
         <v>₹ 31,42,946</v>
@@ -3525,10 +3525,10 @@
         <v>₹ 20,953</v>
       </c>
       <c r="D87" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E87" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F87" t="str">
         <v>₹ 30,98,383</v>
@@ -3548,10 +3548,10 @@
         <v>₹ 20,656</v>
       </c>
       <c r="D88" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E88" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F88" t="str">
         <v>₹ 30,53,522</v>
@@ -3571,10 +3571,10 @@
         <v>₹ 20,357</v>
       </c>
       <c r="D89" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E89" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F89" t="str">
         <v>₹ 30,08,361</v>
@@ -3594,10 +3594,10 @@
         <v>₹ 20,056</v>
       </c>
       <c r="D90" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E90" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F90" t="str">
         <v>₹ 29,62,900</v>
@@ -3617,10 +3617,10 @@
         <v>₹ 19,753</v>
       </c>
       <c r="D91" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E91" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F91" t="str">
         <v>₹ 29,17,136</v>
@@ -3640,10 +3640,10 @@
         <v>₹ 2,12,643</v>
       </c>
       <c r="D92" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E92" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F92" t="str">
         <v>₹ 23,43,576</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>Jan₹ 46,069₹ 19,448₹ 4,250₹ 69,767₹ 28,71,06746.83%Feb₹ 46,376₹ 19,140₹ 4,250₹ 69,767₹ 28,24,69047.69%Mar₹ 46,686₹ 18,831₹ 4,250₹ 69,767₹ 27,78,00548.56%Apr₹ 46,997₹ 18,520₹ 4,250₹ 69,767₹ 27,31,00849.43%May₹ 47,310₹ 18,207₹ 4,250₹ 69,767₹ 26,83,69850.3%Jun₹ 47,626₹ 17,891₹ 4,250₹ 69,767₹ 26,36,07251.18%Jul₹ 47,943₹ 17,574₹ 4,250₹ 69,767₹ 25,88,12952.07%Aug₹ 48,263₹ 17,254₹ 4,250₹ 69,767₹ 25,39,86652.97%Sep₹ 48,584₹ 16,932₹ 4,250₹ 69,767₹ 24,91,28253.87%Oct₹ 48,908₹ 16,609₹ 4,250₹ 69,767₹ 24,42,37354.77%Nov₹ 49,234₹ 16,282₹ 4,250₹ 69,767₹ 23,93,13955.68%Dec₹ 49,563₹ 15,954₹ 4,250₹ 69,767₹ 23,43,57656.6%</v>
+        <v>Jan₹ 46,069₹ 19,448₹ 3,750₹ 69,267₹ 28,71,06746.83%Feb₹ 46,376₹ 19,140₹ 3,750₹ 69,267₹ 28,24,69047.69%Mar₹ 46,686₹ 18,831₹ 3,750₹ 69,267₹ 27,78,00548.56%Apr₹ 46,997₹ 18,520₹ 3,750₹ 69,267₹ 27,31,00849.43%May₹ 47,310₹ 18,207₹ 3,750₹ 69,267₹ 26,83,69850.3%Jun₹ 47,626₹ 17,891₹ 3,750₹ 69,267₹ 26,36,07251.18%Jul₹ 47,943₹ 17,574₹ 3,750₹ 69,267₹ 25,88,12952.07%Aug₹ 48,263₹ 17,254₹ 3,750₹ 69,267₹ 25,39,86652.97%Sep₹ 48,584₹ 16,932₹ 3,750₹ 69,267₹ 24,91,28253.87%Oct₹ 48,908₹ 16,609₹ 3,750₹ 69,267₹ 24,42,37354.77%Nov₹ 49,234₹ 16,282₹ 3,750₹ 69,267₹ 23,93,13955.68%Dec₹ 49,563₹ 15,954₹ 3,750₹ 69,267₹ 23,43,57656.6%</v>
       </c>
       <c r="B93" t="str">
         <v>Jan</v>
@@ -3666,10 +3666,10 @@
         <v>₹ 19,448</v>
       </c>
       <c r="E93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G93" t="str">
         <v>₹ 28,71,067</v>
@@ -3687,10 +3687,10 @@
         <v>₹ 19,140</v>
       </c>
       <c r="L93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N93" t="str">
         <v>₹ 28,24,690</v>
@@ -3708,10 +3708,10 @@
         <v>₹ 18,831</v>
       </c>
       <c r="S93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U93" t="str">
         <v>₹ 27,78,005</v>
@@ -3729,10 +3729,10 @@
         <v>₹ 18,520</v>
       </c>
       <c r="Z93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB93" t="str">
         <v>₹ 27,31,008</v>
@@ -3750,10 +3750,10 @@
         <v>₹ 18,207</v>
       </c>
       <c r="AG93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI93" t="str">
         <v>₹ 26,83,698</v>
@@ -3771,10 +3771,10 @@
         <v>₹ 17,891</v>
       </c>
       <c r="AN93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP93" t="str">
         <v>₹ 26,36,072</v>
@@ -3792,10 +3792,10 @@
         <v>₹ 17,574</v>
       </c>
       <c r="AU93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW93" t="str">
         <v>₹ 25,88,129</v>
@@ -3813,10 +3813,10 @@
         <v>₹ 17,254</v>
       </c>
       <c r="BB93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD93" t="str">
         <v>₹ 25,39,866</v>
@@ -3834,10 +3834,10 @@
         <v>₹ 16,932</v>
       </c>
       <c r="BI93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK93" t="str">
         <v>₹ 24,91,282</v>
@@ -3855,10 +3855,10 @@
         <v>₹ 16,609</v>
       </c>
       <c r="BP93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR93" t="str">
         <v>₹ 24,42,373</v>
@@ -3876,10 +3876,10 @@
         <v>₹ 16,282</v>
       </c>
       <c r="BW93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY93" t="str">
         <v>₹ 23,93,139</v>
@@ -3897,10 +3897,10 @@
         <v>₹ 15,954</v>
       </c>
       <c r="CD93" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE93" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF93" t="str">
         <v>₹ 23,43,576</v>
@@ -3920,10 +3920,10 @@
         <v>₹ 19,448</v>
       </c>
       <c r="D94" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E94" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F94" t="str">
         <v>₹ 28,71,067</v>
@@ -3943,10 +3943,10 @@
         <v>₹ 19,140</v>
       </c>
       <c r="D95" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E95" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F95" t="str">
         <v>₹ 28,24,690</v>
@@ -3966,10 +3966,10 @@
         <v>₹ 18,831</v>
       </c>
       <c r="D96" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E96" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F96" t="str">
         <v>₹ 27,78,005</v>
@@ -3989,10 +3989,10 @@
         <v>₹ 18,520</v>
       </c>
       <c r="D97" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E97" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F97" t="str">
         <v>₹ 27,31,008</v>
@@ -4012,10 +4012,10 @@
         <v>₹ 18,207</v>
       </c>
       <c r="D98" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E98" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F98" t="str">
         <v>₹ 26,83,698</v>
@@ -4035,10 +4035,10 @@
         <v>₹ 17,891</v>
       </c>
       <c r="D99" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E99" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F99" t="str">
         <v>₹ 26,36,072</v>
@@ -4058,10 +4058,10 @@
         <v>₹ 17,574</v>
       </c>
       <c r="D100" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E100" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F100" t="str">
         <v>₹ 25,88,129</v>
@@ -4081,10 +4081,10 @@
         <v>₹ 17,254</v>
       </c>
       <c r="D101" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E101" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F101" t="str">
         <v>₹ 25,39,866</v>
@@ -4104,10 +4104,10 @@
         <v>₹ 16,932</v>
       </c>
       <c r="D102" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E102" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F102" t="str">
         <v>₹ 24,91,282</v>
@@ -4127,10 +4127,10 @@
         <v>₹ 16,609</v>
       </c>
       <c r="D103" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E103" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F103" t="str">
         <v>₹ 24,42,373</v>
@@ -4150,10 +4150,10 @@
         <v>₹ 16,282</v>
       </c>
       <c r="D104" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E104" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F104" t="str">
         <v>₹ 23,93,139</v>
@@ -4173,10 +4173,10 @@
         <v>₹ 15,954</v>
       </c>
       <c r="D105" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E105" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F105" t="str">
         <v>₹ 23,43,576</v>
@@ -4196,10 +4196,10 @@
         <v>₹ 1,65,038</v>
       </c>
       <c r="D106" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E106" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F106" t="str">
         <v>₹ 17,22,411</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>Jan₹ 49,893₹ 15,624₹ 4,250₹ 69,767₹ 22,93,68357.52%Feb₹ 50,226₹ 15,291₹ 4,250₹ 69,767₹ 22,43,45858.45%Mar₹ 50,561₹ 14,956₹ 4,250₹ 69,767₹ 21,92,89759.39%Apr₹ 50,898₹ 14,619₹ 4,250₹ 69,767₹ 21,42,00060.33%May₹ 51,237₹ 14,280₹ 4,250₹ 69,767₹ 20,90,76361.28%Jun₹ 51,578₹ 13,938₹ 4,250₹ 69,767₹ 20,39,18462.24%Jul₹ 51,922₹ 13,595₹ 4,250₹ 69,767₹ 19,87,26263.2%Aug₹ 52,268₹ 13,248₹ 4,250₹ 69,767₹ 19,34,99364.17%Sep₹ 52,617₹ 12,900₹ 4,250₹ 69,767₹ 18,82,37665.14%Oct₹ 52,968₹ 12,549₹ 4,250₹ 69,767₹ 18,29,40966.12%Nov₹ 53,321₹ 12,196₹ 4,250₹ 69,767₹ 17,76,08867.11%Dec₹ 53,676₹ 11,841₹ 4,250₹ 69,767₹ 17,22,41168.1%</v>
+        <v>Jan₹ 49,893₹ 15,624₹ 3,750₹ 69,267₹ 22,93,68357.52%Feb₹ 50,226₹ 15,291₹ 3,750₹ 69,267₹ 22,43,45858.45%Mar₹ 50,561₹ 14,956₹ 3,750₹ 69,267₹ 21,92,89759.39%Apr₹ 50,898₹ 14,619₹ 3,750₹ 69,267₹ 21,42,00060.33%May₹ 51,237₹ 14,280₹ 3,750₹ 69,267₹ 20,90,76361.28%Jun₹ 51,578₹ 13,938₹ 3,750₹ 69,267₹ 20,39,18462.24%Jul₹ 51,922₹ 13,595₹ 3,750₹ 69,267₹ 19,87,26263.2%Aug₹ 52,268₹ 13,248₹ 3,750₹ 69,267₹ 19,34,99364.17%Sep₹ 52,617₹ 12,900₹ 3,750₹ 69,267₹ 18,82,37665.14%Oct₹ 52,968₹ 12,549₹ 3,750₹ 69,267₹ 18,29,40966.12%Nov₹ 53,321₹ 12,196₹ 3,750₹ 69,267₹ 17,76,08867.11%Dec₹ 53,676₹ 11,841₹ 3,750₹ 69,267₹ 17,22,41168.1%</v>
       </c>
       <c r="B107" t="str">
         <v>Jan</v>
@@ -4222,10 +4222,10 @@
         <v>₹ 15,624</v>
       </c>
       <c r="E107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G107" t="str">
         <v>₹ 22,93,683</v>
@@ -4243,10 +4243,10 @@
         <v>₹ 15,291</v>
       </c>
       <c r="L107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N107" t="str">
         <v>₹ 22,43,458</v>
@@ -4264,10 +4264,10 @@
         <v>₹ 14,956</v>
       </c>
       <c r="S107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U107" t="str">
         <v>₹ 21,92,897</v>
@@ -4285,10 +4285,10 @@
         <v>₹ 14,619</v>
       </c>
       <c r="Z107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB107" t="str">
         <v>₹ 21,42,000</v>
@@ -4306,10 +4306,10 @@
         <v>₹ 14,280</v>
       </c>
       <c r="AG107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI107" t="str">
         <v>₹ 20,90,763</v>
@@ -4327,10 +4327,10 @@
         <v>₹ 13,938</v>
       </c>
       <c r="AN107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP107" t="str">
         <v>₹ 20,39,184</v>
@@ -4348,10 +4348,10 @@
         <v>₹ 13,595</v>
       </c>
       <c r="AU107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW107" t="str">
         <v>₹ 19,87,262</v>
@@ -4369,10 +4369,10 @@
         <v>₹ 13,248</v>
       </c>
       <c r="BB107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD107" t="str">
         <v>₹ 19,34,993</v>
@@ -4390,10 +4390,10 @@
         <v>₹ 12,900</v>
       </c>
       <c r="BI107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK107" t="str">
         <v>₹ 18,82,376</v>
@@ -4411,10 +4411,10 @@
         <v>₹ 12,549</v>
       </c>
       <c r="BP107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR107" t="str">
         <v>₹ 18,29,409</v>
@@ -4432,10 +4432,10 @@
         <v>₹ 12,196</v>
       </c>
       <c r="BW107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY107" t="str">
         <v>₹ 17,76,088</v>
@@ -4453,10 +4453,10 @@
         <v>₹ 11,841</v>
       </c>
       <c r="CD107" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE107" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF107" t="str">
         <v>₹ 17,22,411</v>
@@ -4476,10 +4476,10 @@
         <v>₹ 15,624</v>
       </c>
       <c r="D108" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E108" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F108" t="str">
         <v>₹ 22,93,683</v>
@@ -4499,10 +4499,10 @@
         <v>₹ 15,291</v>
       </c>
       <c r="D109" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E109" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F109" t="str">
         <v>₹ 22,43,458</v>
@@ -4522,10 +4522,10 @@
         <v>₹ 14,956</v>
       </c>
       <c r="D110" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E110" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F110" t="str">
         <v>₹ 21,92,897</v>
@@ -4545,10 +4545,10 @@
         <v>₹ 14,619</v>
       </c>
       <c r="D111" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E111" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F111" t="str">
         <v>₹ 21,42,000</v>
@@ -4568,10 +4568,10 @@
         <v>₹ 14,280</v>
       </c>
       <c r="D112" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E112" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F112" t="str">
         <v>₹ 20,90,763</v>
@@ -4591,10 +4591,10 @@
         <v>₹ 13,938</v>
       </c>
       <c r="D113" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E113" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F113" t="str">
         <v>₹ 20,39,184</v>
@@ -4614,10 +4614,10 @@
         <v>₹ 13,595</v>
       </c>
       <c r="D114" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E114" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F114" t="str">
         <v>₹ 19,87,262</v>
@@ -4637,10 +4637,10 @@
         <v>₹ 13,248</v>
       </c>
       <c r="D115" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E115" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F115" t="str">
         <v>₹ 19,34,993</v>
@@ -4660,10 +4660,10 @@
         <v>₹ 12,900</v>
       </c>
       <c r="D116" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E116" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F116" t="str">
         <v>₹ 18,82,376</v>
@@ -4683,10 +4683,10 @@
         <v>₹ 12,549</v>
       </c>
       <c r="D117" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E117" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F117" t="str">
         <v>₹ 18,29,409</v>
@@ -4706,10 +4706,10 @@
         <v>₹ 12,196</v>
       </c>
       <c r="D118" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E118" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F118" t="str">
         <v>₹ 17,76,088</v>
@@ -4729,10 +4729,10 @@
         <v>₹ 11,841</v>
       </c>
       <c r="D119" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E119" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F119" t="str">
         <v>₹ 17,22,411</v>
@@ -4752,10 +4752,10 @@
         <v>₹ 1,13,482</v>
       </c>
       <c r="D120" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E120" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F120" t="str">
         <v>₹ 10,49,690</v>
@@ -4766,7 +4766,7 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>Jan₹ 54,034₹ 11,483₹ 4,250₹ 69,767₹ 16,68,37769.1%Feb₹ 54,394₹ 11,123₹ 4,250₹ 69,767₹ 16,13,98370.11%Mar₹ 54,757₹ 10,760₹ 4,250₹ 69,767₹ 15,59,22671.13%Apr₹ 55,122₹ 10,395₹ 4,250₹ 69,767₹ 15,04,10472.15%May₹ 55,490₹ 10,027₹ 4,250₹ 69,767₹ 14,48,61473.17%Jun₹ 55,859₹ 9,657₹ 4,250₹ 69,767₹ 13,92,75574.21%Jul₹ 56,232₹ 9,285₹ 4,250₹ 69,767₹ 13,36,52375.25%Aug₹ 56,607₹ 8,910₹ 4,250₹ 69,767₹ 12,79,91676.3%Sep₹ 56,984₹ 8,533₹ 4,250₹ 69,767₹ 12,22,93277.35%Oct₹ 57,364₹ 8,153₹ 4,250₹ 69,767₹ 11,65,56878.42%Nov₹ 57,746₹ 7,770₹ 4,250₹ 69,767₹ 11,07,82279.48%Dec₹ 58,131₹ 7,385₹ 4,250₹ 69,767₹ 10,49,69080.56%</v>
+        <v>Jan₹ 54,034₹ 11,483₹ 3,750₹ 69,267₹ 16,68,37769.1%Feb₹ 54,394₹ 11,123₹ 3,750₹ 69,267₹ 16,13,98370.11%Mar₹ 54,757₹ 10,760₹ 3,750₹ 69,267₹ 15,59,22671.13%Apr₹ 55,122₹ 10,395₹ 3,750₹ 69,267₹ 15,04,10472.15%May₹ 55,490₹ 10,027₹ 3,750₹ 69,267₹ 14,48,61473.17%Jun₹ 55,859₹ 9,657₹ 3,750₹ 69,267₹ 13,92,75574.21%Jul₹ 56,232₹ 9,285₹ 3,750₹ 69,267₹ 13,36,52375.25%Aug₹ 56,607₹ 8,910₹ 3,750₹ 69,267₹ 12,79,91676.3%Sep₹ 56,984₹ 8,533₹ 3,750₹ 69,267₹ 12,22,93277.35%Oct₹ 57,364₹ 8,153₹ 3,750₹ 69,267₹ 11,65,56878.42%Nov₹ 57,746₹ 7,770₹ 3,750₹ 69,267₹ 11,07,82279.48%Dec₹ 58,131₹ 7,385₹ 3,750₹ 69,267₹ 10,49,69080.56%</v>
       </c>
       <c r="B121" t="str">
         <v>Jan</v>
@@ -4778,10 +4778,10 @@
         <v>₹ 11,483</v>
       </c>
       <c r="E121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G121" t="str">
         <v>₹ 16,68,377</v>
@@ -4799,10 +4799,10 @@
         <v>₹ 11,123</v>
       </c>
       <c r="L121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N121" t="str">
         <v>₹ 16,13,983</v>
@@ -4820,10 +4820,10 @@
         <v>₹ 10,760</v>
       </c>
       <c r="S121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U121" t="str">
         <v>₹ 15,59,226</v>
@@ -4841,10 +4841,10 @@
         <v>₹ 10,395</v>
       </c>
       <c r="Z121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB121" t="str">
         <v>₹ 15,04,104</v>
@@ -4862,10 +4862,10 @@
         <v>₹ 10,027</v>
       </c>
       <c r="AG121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI121" t="str">
         <v>₹ 14,48,614</v>
@@ -4883,10 +4883,10 @@
         <v>₹ 9,657</v>
       </c>
       <c r="AN121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP121" t="str">
         <v>₹ 13,92,755</v>
@@ -4904,10 +4904,10 @@
         <v>₹ 9,285</v>
       </c>
       <c r="AU121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW121" t="str">
         <v>₹ 13,36,523</v>
@@ -4925,10 +4925,10 @@
         <v>₹ 8,910</v>
       </c>
       <c r="BB121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD121" t="str">
         <v>₹ 12,79,916</v>
@@ -4946,10 +4946,10 @@
         <v>₹ 8,533</v>
       </c>
       <c r="BI121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK121" t="str">
         <v>₹ 12,22,932</v>
@@ -4967,10 +4967,10 @@
         <v>₹ 8,153</v>
       </c>
       <c r="BP121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR121" t="str">
         <v>₹ 11,65,568</v>
@@ -4988,10 +4988,10 @@
         <v>₹ 7,770</v>
       </c>
       <c r="BW121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY121" t="str">
         <v>₹ 11,07,822</v>
@@ -5009,10 +5009,10 @@
         <v>₹ 7,385</v>
       </c>
       <c r="CD121" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE121" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF121" t="str">
         <v>₹ 10,49,690</v>
@@ -5032,10 +5032,10 @@
         <v>₹ 11,483</v>
       </c>
       <c r="D122" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E122" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F122" t="str">
         <v>₹ 16,68,377</v>
@@ -5055,10 +5055,10 @@
         <v>₹ 11,123</v>
       </c>
       <c r="D123" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E123" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F123" t="str">
         <v>₹ 16,13,983</v>
@@ -5078,10 +5078,10 @@
         <v>₹ 10,760</v>
       </c>
       <c r="D124" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E124" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F124" t="str">
         <v>₹ 15,59,226</v>
@@ -5101,10 +5101,10 @@
         <v>₹ 10,395</v>
       </c>
       <c r="D125" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E125" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F125" t="str">
         <v>₹ 15,04,104</v>
@@ -5124,10 +5124,10 @@
         <v>₹ 10,027</v>
       </c>
       <c r="D126" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E126" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F126" t="str">
         <v>₹ 14,48,614</v>
@@ -5147,10 +5147,10 @@
         <v>₹ 9,657</v>
       </c>
       <c r="D127" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E127" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F127" t="str">
         <v>₹ 13,92,755</v>
@@ -5170,10 +5170,10 @@
         <v>₹ 9,285</v>
       </c>
       <c r="D128" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E128" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F128" t="str">
         <v>₹ 13,36,523</v>
@@ -5193,10 +5193,10 @@
         <v>₹ 8,910</v>
       </c>
       <c r="D129" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E129" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F129" t="str">
         <v>₹ 12,79,916</v>
@@ -5216,10 +5216,10 @@
         <v>₹ 8,533</v>
       </c>
       <c r="D130" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E130" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F130" t="str">
         <v>₹ 12,22,932</v>
@@ -5239,10 +5239,10 @@
         <v>₹ 8,153</v>
       </c>
       <c r="D131" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E131" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F131" t="str">
         <v>₹ 11,65,568</v>
@@ -5262,10 +5262,10 @@
         <v>₹ 7,770</v>
       </c>
       <c r="D132" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E132" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F132" t="str">
         <v>₹ 11,07,822</v>
@@ -5285,10 +5285,10 @@
         <v>₹ 7,385</v>
       </c>
       <c r="D133" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E133" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F133" t="str">
         <v>₹ 10,49,690</v>
@@ -5308,10 +5308,10 @@
         <v>₹ 57,646</v>
       </c>
       <c r="D134" t="str">
-        <v>₹ 51,000</v>
+        <v>₹ 45,000</v>
       </c>
       <c r="E134" t="str">
-        <v>₹ 8,37,203</v>
+        <v>₹ 8,31,203</v>
       </c>
       <c r="F134" t="str">
         <v>₹ 3,21,133</v>
@@ -5322,7 +5322,7 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>Jan₹ 58,519₹ 6,998₹ 4,250₹ 69,767₹ 9,91,17181.64%Feb₹ 58,909₹ 6,608₹ 4,250₹ 69,767₹ 9,32,26282.74%Mar₹ 59,302₹ 6,215₹ 4,250₹ 69,767₹ 8,72,96083.83%Apr₹ 59,697₹ 5,820₹ 4,250₹ 69,767₹ 8,13,26384.94%May₹ 60,095₹ 5,422₹ 4,250₹ 69,767₹ 7,53,16886.05%Jun₹ 60,496₹ 5,021₹ 4,250₹ 69,767₹ 6,92,67287.17%Jul₹ 60,899₹ 4,618₹ 4,250₹ 69,767₹ 6,31,77388.3%Aug₹ 61,305₹ 4,212₹ 4,250₹ 69,767₹ 5,70,46889.44%Sep₹ 61,714₹ 3,803₹ 4,250₹ 69,767₹ 5,08,75490.58%Oct₹ 62,125₹ 3,392₹ 4,250₹ 69,767₹ 4,46,62991.73%Nov₹ 62,539₹ 2,978₹ 4,250₹ 69,767₹ 3,84,09092.89%Dec₹ 62,956₹ 2,561₹ 4,250₹ 69,767₹ 3,21,13394.05%</v>
+        <v>Jan₹ 58,519₹ 6,998₹ 3,750₹ 69,267₹ 9,91,17181.64%Feb₹ 58,909₹ 6,608₹ 3,750₹ 69,267₹ 9,32,26282.74%Mar₹ 59,302₹ 6,215₹ 3,750₹ 69,267₹ 8,72,96083.83%Apr₹ 59,697₹ 5,820₹ 3,750₹ 69,267₹ 8,13,26384.94%May₹ 60,095₹ 5,422₹ 3,750₹ 69,267₹ 7,53,16886.05%Jun₹ 60,496₹ 5,021₹ 3,750₹ 69,267₹ 6,92,67287.17%Jul₹ 60,899₹ 4,618₹ 3,750₹ 69,267₹ 6,31,77388.3%Aug₹ 61,305₹ 4,212₹ 3,750₹ 69,267₹ 5,70,46889.44%Sep₹ 61,714₹ 3,803₹ 3,750₹ 69,267₹ 5,08,75490.58%Oct₹ 62,125₹ 3,392₹ 3,750₹ 69,267₹ 4,46,62991.73%Nov₹ 62,539₹ 2,978₹ 3,750₹ 69,267₹ 3,84,09092.89%Dec₹ 62,956₹ 2,561₹ 3,750₹ 69,267₹ 3,21,13394.05%</v>
       </c>
       <c r="B135" t="str">
         <v>Jan</v>
@@ -5334,10 +5334,10 @@
         <v>₹ 6,998</v>
       </c>
       <c r="E135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G135" t="str">
         <v>₹ 9,91,171</v>
@@ -5355,10 +5355,10 @@
         <v>₹ 6,608</v>
       </c>
       <c r="L135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N135" t="str">
         <v>₹ 9,32,262</v>
@@ -5376,10 +5376,10 @@
         <v>₹ 6,215</v>
       </c>
       <c r="S135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U135" t="str">
         <v>₹ 8,72,960</v>
@@ -5397,10 +5397,10 @@
         <v>₹ 5,820</v>
       </c>
       <c r="Z135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB135" t="str">
         <v>₹ 8,13,263</v>
@@ -5418,10 +5418,10 @@
         <v>₹ 5,422</v>
       </c>
       <c r="AG135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI135" t="str">
         <v>₹ 7,53,168</v>
@@ -5439,10 +5439,10 @@
         <v>₹ 5,021</v>
       </c>
       <c r="AN135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AO135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AP135" t="str">
         <v>₹ 6,92,672</v>
@@ -5460,10 +5460,10 @@
         <v>₹ 4,618</v>
       </c>
       <c r="AU135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AV135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AW135" t="str">
         <v>₹ 6,31,773</v>
@@ -5481,10 +5481,10 @@
         <v>₹ 4,212</v>
       </c>
       <c r="BB135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BC135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BD135" t="str">
         <v>₹ 5,70,468</v>
@@ -5502,10 +5502,10 @@
         <v>₹ 3,803</v>
       </c>
       <c r="BI135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BJ135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BK135" t="str">
         <v>₹ 5,08,754</v>
@@ -5523,10 +5523,10 @@
         <v>₹ 3,392</v>
       </c>
       <c r="BP135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BQ135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BR135" t="str">
         <v>₹ 4,46,629</v>
@@ -5544,10 +5544,10 @@
         <v>₹ 2,978</v>
       </c>
       <c r="BW135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="BX135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="BY135" t="str">
         <v>₹ 3,84,090</v>
@@ -5565,10 +5565,10 @@
         <v>₹ 2,561</v>
       </c>
       <c r="CD135" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="CE135" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="CF135" t="str">
         <v>₹ 3,21,133</v>
@@ -5588,10 +5588,10 @@
         <v>₹ 6,998</v>
       </c>
       <c r="D136" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E136" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F136" t="str">
         <v>₹ 9,91,171</v>
@@ -5611,10 +5611,10 @@
         <v>₹ 6,608</v>
       </c>
       <c r="D137" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E137" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F137" t="str">
         <v>₹ 9,32,262</v>
@@ -5634,10 +5634,10 @@
         <v>₹ 6,215</v>
       </c>
       <c r="D138" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E138" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F138" t="str">
         <v>₹ 8,72,960</v>
@@ -5657,10 +5657,10 @@
         <v>₹ 5,820</v>
       </c>
       <c r="D139" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E139" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F139" t="str">
         <v>₹ 8,13,263</v>
@@ -5680,10 +5680,10 @@
         <v>₹ 5,422</v>
       </c>
       <c r="D140" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E140" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F140" t="str">
         <v>₹ 7,53,168</v>
@@ -5703,10 +5703,10 @@
         <v>₹ 5,021</v>
       </c>
       <c r="D141" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E141" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F141" t="str">
         <v>₹ 6,92,672</v>
@@ -5726,10 +5726,10 @@
         <v>₹ 4,618</v>
       </c>
       <c r="D142" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E142" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F142" t="str">
         <v>₹ 6,31,773</v>
@@ -5749,10 +5749,10 @@
         <v>₹ 4,212</v>
       </c>
       <c r="D143" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E143" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F143" t="str">
         <v>₹ 5,70,468</v>
@@ -5772,10 +5772,10 @@
         <v>₹ 3,803</v>
       </c>
       <c r="D144" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E144" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F144" t="str">
         <v>₹ 5,08,754</v>
@@ -5795,10 +5795,10 @@
         <v>₹ 3,392</v>
       </c>
       <c r="D145" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E145" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F145" t="str">
         <v>₹ 4,46,629</v>
@@ -5818,10 +5818,10 @@
         <v>₹ 2,978</v>
       </c>
       <c r="D146" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E146" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F146" t="str">
         <v>₹ 3,84,090</v>
@@ -5841,10 +5841,10 @@
         <v>₹ 2,561</v>
       </c>
       <c r="D147" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E147" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F147" t="str">
         <v>₹ 3,21,133</v>
@@ -5864,10 +5864,10 @@
         <v>₹ 6,451</v>
       </c>
       <c r="D148" t="str">
-        <v>₹ 21,250</v>
+        <v>₹ 18,750</v>
       </c>
       <c r="E148" t="str">
-        <v>₹ 3,48,835</v>
+        <v>₹ 3,46,335</v>
       </c>
       <c r="F148" t="str">
         <v>₹ 0</v>
@@ -5878,7 +5878,7 @@
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>Jan₹ 63,376₹ 2,141₹ 4,250₹ 69,767₹ 2,57,75795.23%Feb₹ 63,799₹ 1,718₹ 4,250₹ 69,767₹ 1,93,95996.41%Mar₹ 64,224₹ 1,293₹ 4,250₹ 69,767₹ 1,29,73597.6%Apr₹ 64,652₹ 865₹ 4,250₹ 69,767₹ 65,08398.79%May₹ 65,083₹ 434₹ 4,250₹ 69,767₹ 0100%</v>
+        <v>Jan₹ 63,376₹ 2,141₹ 3,750₹ 69,267₹ 2,57,75795.23%Feb₹ 63,799₹ 1,718₹ 3,750₹ 69,267₹ 1,93,95996.41%Mar₹ 64,224₹ 1,293₹ 3,750₹ 69,267₹ 1,29,73597.6%Apr₹ 64,652₹ 865₹ 3,750₹ 69,267₹ 65,08398.79%May₹ 65,083₹ 434₹ 3,750₹ 69,267₹ 0100%</v>
       </c>
       <c r="B149" t="str">
         <v>Jan</v>
@@ -5890,10 +5890,10 @@
         <v>₹ 2,141</v>
       </c>
       <c r="E149" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="F149" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="G149" t="str">
         <v>₹ 2,57,757</v>
@@ -5911,10 +5911,10 @@
         <v>₹ 1,718</v>
       </c>
       <c r="L149" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="M149" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="N149" t="str">
         <v>₹ 1,93,959</v>
@@ -5932,10 +5932,10 @@
         <v>₹ 1,293</v>
       </c>
       <c r="S149" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="T149" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="U149" t="str">
         <v>₹ 1,29,735</v>
@@ -5953,10 +5953,10 @@
         <v>₹ 865</v>
       </c>
       <c r="Z149" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AA149" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AB149" t="str">
         <v>₹ 65,083</v>
@@ -5974,10 +5974,10 @@
         <v>₹ 434</v>
       </c>
       <c r="AG149" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="AH149" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="AI149" t="str">
         <v>₹ 0</v>
@@ -5997,10 +5997,10 @@
         <v>₹ 2,141</v>
       </c>
       <c r="D150" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E150" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F150" t="str">
         <v>₹ 2,57,757</v>
@@ -6020,10 +6020,10 @@
         <v>₹ 1,718</v>
       </c>
       <c r="D151" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E151" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F151" t="str">
         <v>₹ 1,93,959</v>
@@ -6043,10 +6043,10 @@
         <v>₹ 1,293</v>
       </c>
       <c r="D152" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E152" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F152" t="str">
         <v>₹ 1,29,735</v>
@@ -6066,10 +6066,10 @@
         <v>₹ 865</v>
       </c>
       <c r="D153" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E153" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F153" t="str">
         <v>₹ 65,083</v>
@@ -6089,10 +6089,10 @@
         <v>₹ 434</v>
       </c>
       <c r="D154" t="str">
-        <v>₹ 4,250</v>
+        <v>₹ 3,750</v>
       </c>
       <c r="E154" t="str">
-        <v>₹ 69,767</v>
+        <v>₹ 69,267</v>
       </c>
       <c r="F154" t="str">
         <v>₹ 0</v>

</xml_diff>